<commit_message>
Update test data to fix failing test
</commit_message>
<xml_diff>
--- a/tests/services/data/pbmc_non_existing_trial.xlsx
+++ b/tests/services/data/pbmc_non_existing_trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-api-gae/tests/services/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-api-gae/tests/services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF4598E-A4B7-FA4E-9147-D63087B83D61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6121C87-6E7C-5F45-B373-D17678D89FC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="8300" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shipment" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -57,7 +57,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -70,7 +70,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -165,7 +165,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
+          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
         </r>
       </text>
     </comment>
@@ -178,7 +178,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shipment made.</t>
+          <t>Type of shippment made.</t>
         </r>
       </text>
     </comment>
@@ -270,12 +270,12 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{71E59CFE-AA76-8142-B2A2-03FE06C23FD8}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{EB3386D3-F9F1-E74C-9496-E6019BF93F5E}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -283,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{225E9DBC-E3A9-BA46-A7B7-5B6B08C8CF46}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{1E3CE706-B650-5C47-BC63-E6934412A65B}">
       <text>
         <r>
           <rPr>
@@ -296,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{B0B48A2B-6506-9846-978D-9F56864750F6}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{4560212F-781B-BB4A-9DC3-A564D1CF42B9}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{1CB30327-1AC0-A04A-9ADC-B22B3C49C9B5}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{34F062A5-F241-EC43-ABFB-9C226DF66B93}">
       <text>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{9DB4E4E4-9552-7E4F-B4C7-606BD72B08D8}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{5E0CE324-AE1E-714E-9BF4-2F95750CE31F}">
       <text>
         <r>
           <rPr>
@@ -335,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{80275666-DDAE-2A4A-A5BA-C940328AF719}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{0C7B6D22-DAB9-C942-8215-1728F79BEC8A}">
       <text>
         <r>
           <rPr>
@@ -348,12 +348,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{D904260A-6685-7640-AC36-F0A46D4C19AB}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{B950FFD6-75B8-DB4E-84DF-98BC0BFEEE5C}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -361,12 +361,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{8087506B-BCFA-2B4B-9E2F-DD1D7C2AF187}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{F3982C5C-3395-2D44-9037-112C89905579}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -374,7 +374,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{F8132DDC-108E-554C-ADC4-A527A5933184}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{1BF979EC-C2A0-F045-9D1A-8F7634F1B5B1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{59E607CB-D60E-314E-B8CA-F9ABCDC5AD11}">
       <text>
         <r>
           <rPr>
@@ -387,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{8CDB0C62-7488-0A49-986B-89A21FB1D694}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{D27C61C4-C974-8F4C-88B9-C18272BA2BED}">
       <text>
         <r>
           <rPr>
@@ -400,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7288029F-DAF7-3341-A192-9300FF34B56B}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{03677D58-45DA-024D-ACFF-8D696CBAD0D1}">
       <text>
         <r>
           <rPr>
@@ -413,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{0EEB60B7-23C1-4143-85EB-F1EB272F49C4}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{CA540AFF-9784-FC4C-9272-48911F67FBCC}">
       <text>
         <r>
           <rPr>
@@ -426,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D62D6863-CB88-C94B-9783-BEF16D0F8EEA}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{AA420F68-B01F-EA48-82B7-9D9670CA86CE}">
       <text>
         <r>
           <rPr>
@@ -439,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{FB7A73F1-797D-5741-83DA-079D906DB76A}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{223E686F-EE26-9144-A7EE-83E84FC2376B}">
       <text>
         <r>
           <rPr>
@@ -452,7 +465,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{53948CAA-53F1-594A-942D-B4F788EE28B4}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{32B8B1ED-3C64-964B-9AFE-A7DE2F2CF21C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quantity of each sample shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{5A3C01C8-44A9-2A47-816F-558201139159}">
       <text>
         <r>
           <rPr>
@@ -461,11 +487,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each aliquot shipped.</t>
+          <t>Volume of sample shipped.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{D02E2AE2-3A7A-034B-A336-2AF3CA35B1FA}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{16D56719-31FE-F448-8360-54B72A0E88A6}">
       <text>
         <r>
           <rPr>
@@ -474,24 +500,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of aliquot shipped.</t>
+          <t>The unit of biological material from this sample.</t>
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{D3E102DC-A8D7-F74C-8D6D-B407FB535CE9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The unit of biological material from this aliquot.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{7622B2CB-7D7B-1F46-92C7-9C3DEA932538}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{49AC0293-F3FA-0B4E-A9B3-F83AF5B676B1}">
       <text>
         <r>
           <rPr>
@@ -504,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{B84EBF1B-8DCE-624A-A8A3-C5F610F15733}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{C5E1A3A3-0A7A-A14D-9616-14E5C04DF0FA}">
       <text>
         <r>
           <rPr>
@@ -517,12 +530,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{1B9BB21E-23FF-FA4F-BC90-532ADB8205BF}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{C72612C5-E521-D744-A104-8C1AC39BA4FB}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -530,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{7B80F8AE-0376-D941-91FE-4D27909E8DD4}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{BDB79CA7-39FF-3D47-8F60-E617144A0B5F}">
       <text>
         <r>
           <rPr>
@@ -543,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{FCBAF0CC-6893-634E-BCB7-6218EED21E97}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{002EDB75-E83C-2C4B-98EC-02FA37990436}">
       <text>
         <r>
           <rPr>
@@ -556,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{CBE7FC9C-0772-7449-9637-1B4338BD258B}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{F5195E2B-2714-3E4B-B63B-44BF9029B783}">
       <text>
         <r>
           <rPr>
@@ -569,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{B8A82EAD-78B2-014A-BAB5-1262D806D483}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{0978C15D-8CF0-6A43-8247-F9127B506BE8}">
       <text>
         <r>
           <rPr>
@@ -578,33 +591,33 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of aliquot after QC and pathology review.</t>
+          <t>Final status of sample after QC and pathology review.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{D6D823C3-E025-8C4B-AD66-E5CF96C2E6D8}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{8952E4A9-B5E8-9340-88B4-5BCE85C9CC51}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of aliquot if replacement is/was requested.</t>
+          <t>Status of sample if replacement is/was requested.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{E40FCBF1-69F7-F344-9995-EAB202F1570B}">
+    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{16BCC139-A77A-DC40-85C3-D74D57ECCC35}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of aliquot used for other assay, exhausted, destroyed, or returned.</t>
+          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -613,7 +626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="88">
   <si>
     <t>#t</t>
   </si>
@@ -804,24 +817,6 @@
     <t>FFPE block #52</t>
   </si>
   <si>
-    <t>CIMAC-12345</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
-  </si>
-  <si>
     <t>Usable for Assay</t>
   </si>
   <si>
@@ -831,16 +826,70 @@
     <t>Other</t>
   </si>
   <si>
+    <t>tPA1</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA1SA1</t>
+  </si>
+  <si>
+    <t>tPA2</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA2SA2</t>
+  </si>
+  <si>
+    <t>PA1SA1-al1</t>
+  </si>
+  <si>
+    <t>PA1SA1-al2</t>
+  </si>
+  <si>
+    <t>PA2SA2-al6</t>
+  </si>
+  <si>
+    <t>GENOMIC SOURCE</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Progression</t>
+  </si>
+  <si>
+    <t>PA1SA2</t>
+  </si>
+  <si>
+    <t>PA2SA1</t>
+  </si>
+  <si>
+    <t>PA1SA2-al3</t>
+  </si>
+  <si>
+    <t>PA2SA1-al4</t>
+  </si>
+  <si>
+    <t>PA2SA1-al5</t>
+  </si>
+  <si>
+    <t>ALIQUOT QUALITY STATUS</t>
+  </si>
+  <si>
+    <t>ALIQUOT REPLACEMENT</t>
+  </si>
+  <si>
+    <t>ALIQUOT STATUS</t>
+  </si>
+  <si>
     <t>test-non-existing-trial-id</t>
-  </si>
-  <si>
-    <t>ALIQUOT QUALITY STATUS</t>
-  </si>
-  <si>
-    <t>ALIQUOT REPLACEMENT</t>
-  </si>
-  <si>
-    <t>ALIQUOT STATUS</t>
   </si>
 </sst>
 </file>
@@ -902,7 +951,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -936,11 +985,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -953,8 +1039,25 @@
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1295,11 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA212"/>
+  <dimension ref="A1:AB219"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1308,40 +1410,41 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-    </row>
-    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+    </row>
+    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1349,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1375,8 +1478,9 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-    </row>
-    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1410,8 +1514,9 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1445,8 +1550,9 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1480,8 +1586,9 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-    </row>
-    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1515,8 +1622,9 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-    </row>
-    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1550,8 +1658,9 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-    </row>
-    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1585,8 +1694,9 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1620,8 +1730,9 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-    </row>
-    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1655,8 +1766,9 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1690,8 +1802,9 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1725,8 +1838,9 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1760,8 +1874,9 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-    </row>
-    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1795,8 +1910,9 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-    </row>
-    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1830,8 +1946,9 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-    </row>
-    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1865,8 +1982,9 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1900,8 +2018,9 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-    </row>
-    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB17" s="1"/>
+    </row>
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1935,8 +2054,9 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1970,68 +2090,54 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB19" s="1"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -2936,47 +3042,85 @@
         <v>24</v>
       </c>
     </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:AA1"/>
+    <mergeCell ref="B1:AB1"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{F3E6FE57-72BC-A740-8715-EFC67E4B4A18}">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{CEF4F657-9B17-3D4E-BEB7-AA512C805C9E}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF5C08EF-F396-B04E-BDB1-A22098E080AA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{0508AC2A-D608-2742-B360-C6BD4B978327}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D6766716-97CD-D448-8D73-8476497F5B74}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{8F51FE5D-A049-2647-AF9A-9F996C2231EE}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{9BC69022-A0AD-C645-82ED-2DA1E8EE9692}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{39FEEF23-CBE4-7248-97CE-A76CCDCB9339}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K20:K212 I20:I212" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(I20:I219),LEFT(CELL("format",I20:I219),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L26:L219 J26:J219" xr:uid="{142A586A-7C9A-294A-8DFF-BD228EAC837D}">
+      <formula1>AND(ISNUMBER(J26:J225),LEFT(CELL("format",J26:J225),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L20:L212 J20:J212" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M26:M219 K26:K219 L21:L25 J21:J25" xr:uid="{A4734441-4211-D745-B6D2-9CC614A9576C}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N20:N212" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O26:O219 N21:N25" xr:uid="{37B7A701-9B24-054D-8D31-F47801122FEE}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O20:O212" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P26:P219 O21:O25" xr:uid="{70D0F074-FC4B-B942-97DE-D4A2D4E1391D}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R20:R212" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S26:S219 R21:R25" xr:uid="{5F1B1B1D-ACF3-144C-BDFE-5A40FF86BF7F}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y20:Y212" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z26:Z219 Y21:Y25" xr:uid="{EFDA8D82-62D3-914F-95CC-94B96EE5BD9F}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z20:Z212" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA26:AA219 Z21:Z25" xr:uid="{62F7AA30-EDCF-A344-959F-99FE519F4AF1}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA20:AA212" xr:uid="{00000000-0002-0000-0000-00000D000000}">
-      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB26:AB219 AA21:AA25" xr:uid="{CCA786E5-3820-964D-9D71-23F86EFA5623}">
+      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K21:K25 I21:I25" xr:uid="{1C904381-45E6-E043-A765-F11CB6C61550}">
+      <formula1>AND(ISNUMBER(J21:J220),LEFT(CELL("format",J21:J220),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2985,12 +3129,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F096212-B8F8-8645-90B3-5518361EA01E}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AA202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B9C197-8600-D943-8391-ECAEAF59EB82}">
+  <dimension ref="A2:AB203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2999,213 +3142,134 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="12"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <v>54321</v>
-      </c>
-      <c r="C3">
-        <v>12345</v>
-      </c>
-      <c r="D3">
-        <v>54321</v>
-      </c>
-      <c r="E3">
-        <v>12345</v>
-      </c>
-      <c r="F3">
-        <v>54321</v>
-      </c>
-      <c r="G3">
-        <v>12345</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K3">
-        <v>41193</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3">
-        <v>100</v>
-      </c>
-      <c r="Q3">
-        <v>100</v>
-      </c>
-      <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3">
-        <v>10</v>
-      </c>
-      <c r="T3" t="s">
-        <v>62</v>
-      </c>
-      <c r="U3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V3">
-        <v>123</v>
-      </c>
-      <c r="W3">
-        <v>122</v>
-      </c>
-      <c r="X3">
-        <v>100</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4">
-        <v>54321</v>
-      </c>
-      <c r="C4">
-        <v>12345</v>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
       </c>
       <c r="D4">
         <v>54321</v>
@@ -3216,79 +3280,82 @@
       <c r="F4">
         <v>54321</v>
       </c>
-      <c r="G4">
-        <v>12345</v>
+      <c r="G4" t="s">
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4">
+        <v>41193</v>
+      </c>
+      <c r="K4" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>41193</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>58</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>59</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>60</v>
-      </c>
-      <c r="P4">
-        <v>100</v>
       </c>
       <c r="Q4">
         <v>100</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4" t="s">
         <v>61</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>10</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>62</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4">
+        <v>123</v>
+      </c>
+      <c r="X4">
+        <v>122</v>
+      </c>
+      <c r="Y4">
+        <v>100</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" t="s">
         <v>64</v>
       </c>
-      <c r="V4">
-        <v>123</v>
-      </c>
-      <c r="W4">
-        <v>122</v>
-      </c>
-      <c r="X4">
-        <v>100</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5">
-        <v>54321</v>
-      </c>
-      <c r="C5">
-        <v>12345</v>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
       </c>
       <c r="D5">
         <v>54321</v>
@@ -3299,79 +3366,82 @@
       <c r="F5">
         <v>54321</v>
       </c>
-      <c r="G5">
-        <v>12345</v>
+      <c r="G5" t="s">
+        <v>68</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5">
+        <v>41193</v>
+      </c>
+      <c r="K5" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>41193</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>58</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>59</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>60</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
       </c>
       <c r="Q5">
         <v>100</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5" t="s">
         <v>61</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>10</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>62</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
+        <v>73</v>
+      </c>
+      <c r="W5">
+        <v>123</v>
+      </c>
+      <c r="X5">
+        <v>122</v>
+      </c>
+      <c r="Y5">
+        <v>100</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" t="s">
         <v>65</v>
       </c>
-      <c r="V5">
-        <v>123</v>
-      </c>
-      <c r="W5">
-        <v>122</v>
-      </c>
-      <c r="X5">
-        <v>100</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6">
-        <v>54321</v>
-      </c>
-      <c r="C6">
-        <v>12345</v>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
       </c>
       <c r="D6">
         <v>54321</v>
@@ -3382,79 +3452,82 @@
       <c r="F6">
         <v>54321</v>
       </c>
-      <c r="G6">
-        <v>12345</v>
+      <c r="G6" t="s">
+        <v>79</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J6" s="5">
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6">
+        <v>41193</v>
+      </c>
+      <c r="K6" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>41193</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>58</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>59</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>60</v>
-      </c>
-      <c r="P6">
-        <v>100</v>
       </c>
       <c r="Q6">
         <v>100</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6" t="s">
         <v>61</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>10</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>62</v>
       </c>
-      <c r="U6" t="s">
-        <v>66</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>81</v>
+      </c>
+      <c r="W6">
         <v>123</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>122</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>100</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="C7" t="s">
         <v>70</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
-        <v>54321</v>
-      </c>
-      <c r="C7">
-        <v>12345</v>
       </c>
       <c r="D7">
         <v>54321</v>
@@ -3465,79 +3538,82 @@
       <c r="F7">
         <v>54321</v>
       </c>
-      <c r="G7">
-        <v>12345</v>
+      <c r="G7" t="s">
+        <v>80</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7">
+        <v>41193</v>
+      </c>
+      <c r="K7" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>41193</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>58</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>59</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>60</v>
-      </c>
-      <c r="P7">
-        <v>100</v>
       </c>
       <c r="Q7">
         <v>100</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7" t="s">
         <v>61</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>10</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>62</v>
       </c>
-      <c r="U7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>82</v>
+      </c>
+      <c r="W7">
         <v>123</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>122</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>100</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>69</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="C8" t="s">
         <v>70</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>54321</v>
-      </c>
-      <c r="C8">
-        <v>12345</v>
       </c>
       <c r="D8">
         <v>54321</v>
@@ -3548,106 +3624,190 @@
       <c r="F8">
         <v>54321</v>
       </c>
-      <c r="G8">
-        <v>12345</v>
+      <c r="G8" t="s">
+        <v>80</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="6">
-        <v>33234</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="I8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8">
+        <v>41193</v>
+      </c>
+      <c r="K8" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>41193</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M8" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>58</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>59</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>60</v>
-      </c>
-      <c r="P8">
-        <v>100</v>
       </c>
       <c r="Q8">
         <v>100</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8" t="s">
         <v>61</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>10</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>62</v>
       </c>
-      <c r="U8" t="s">
-        <v>68</v>
-      </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>83</v>
+      </c>
+      <c r="W8">
         <v>123</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>122</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>100</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="C9" t="s">
         <v>70</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="D9">
+        <v>54321</v>
+      </c>
+      <c r="E9">
+        <v>12345</v>
+      </c>
+      <c r="F9">
+        <v>54321</v>
+      </c>
+      <c r="G9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9">
+        <v>41193</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="L9">
+        <v>41193</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>100</v>
+      </c>
+      <c r="S9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9">
+        <v>10</v>
+      </c>
+      <c r="U9" t="s">
+        <v>62</v>
+      </c>
+      <c r="V9" t="s">
+        <v>74</v>
+      </c>
+      <c r="W9">
+        <v>123</v>
+      </c>
+      <c r="X9">
+        <v>122</v>
+      </c>
+      <c r="Y9">
+        <v>100</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -4582,40 +4742,46 @@
         <v>24</v>
       </c>
     </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="V2:AB2"/>
   </mergeCells>
-  <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA8" xr:uid="{F1C69A85-5E53-3344-A5B4-61E17CD8CAB1}">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB4:AB203" xr:uid="{973DDE31-29F8-3946-9F57-C350CEE2F8E5}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202" xr:uid="{2E778AC8-49C9-2F44-AC60-DBE0A8F348C8}">
-      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{5F9E2111-E888-A144-92B3-29BF3F21C820}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA4:AA203" xr:uid="{53B89728-DB3D-7146-83FC-81A0423FBB10}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y202" xr:uid="{D9B9ECAB-8EB3-284C-8269-2AA4D259F44C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4:Z203" xr:uid="{8A57EB6E-B549-7F41-95CA-058366A210CA}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R202" xr:uid="{82DF58DC-30B5-F648-A58F-125ED00B7216}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4:S203" xr:uid="{FDA9BFC4-3089-D140-8BAB-994C4312A18E}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O202" xr:uid="{B7318B68-EDBE-1742-BFA6-821A119DB301}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P203" xr:uid="{B8785C88-AD14-6A42-AC09-8E7503E8BCF8}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202" xr:uid="{F9241F38-D4F5-1342-8A90-95006B344183}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O203" xr:uid="{4BF5B0E7-5C7E-524F-8090-D912731210DB}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L3:L202 J3:J202" xr:uid="{50D5E122-54BD-AA4E-A9EB-D7ABEFAB5005}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M4:M203 K4:K203" xr:uid="{A9095E68-E922-DE4F-8BE7-39F9D59C1209}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K3:K202 I3:I202" xr:uid="{CAD9ACD2-6EF9-FB49-89F3-892AF85486CC}">
-      <formula1>AND(ISNUMBER(I3:I202),LEFT(CELL("format",I3:I202),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L4:L9 J4:J9" xr:uid="{942F830A-8796-0B47-89A8-B18B970FCC09}">
+      <formula1>AND(ISNUMBER(K4:K203),LEFT(CELL("format",K4:K203),1)="D")</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L10:L203 J10:J203" xr:uid="{74A534CB-251F-744A-AD1F-2EBE6269F401}">
+      <formula1>AND(ISNUMBER(J10:J209),LEFT(CELL("format",J10:J209),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="I4:I9" xr:uid="{24F77C24-115C-0447-B2E9-CDD51E4EB709}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>